<commit_message>
started revising schematic and specifying components.
</commit_message>
<xml_diff>
--- a/pcb/stereo-sync-pcb-bom.xlsx
+++ b/pcb/stereo-sync-pcb-bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\eit\mak\20190613-stereo-sync-pcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f002r5k\GitHub\binary-counter\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA03FA20-3468-486B-A171-C73992A65943}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE348F5A-5067-4A8B-AB78-67BCAD7169C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{BFAAAD16-CEC3-4355-83C2-768A17E1DB88}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{BFAAAD16-CEC3-4355-83C2-768A17E1DB88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
   <si>
     <t>DigiKey Part</t>
   </si>
@@ -58,6 +58,183 @@
   </si>
   <si>
     <t>1080-1184-ND</t>
+  </si>
+  <si>
+    <t>609-6366-ND</t>
+  </si>
+  <si>
+    <t>Mfgr. Part</t>
+  </si>
+  <si>
+    <t>54202-G3003LF</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
+    <t>LED Array</t>
+  </si>
+  <si>
+    <t>Programming header</t>
+  </si>
+  <si>
+    <t>Surface Mount LED</t>
+  </si>
+  <si>
+    <t>160-1405-1-ND</t>
+  </si>
+  <si>
+    <t>Mfgr.</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>LTST-C150KRKT</t>
+  </si>
+  <si>
+    <t>Lite-On</t>
+  </si>
+  <si>
+    <t>ATXMEGA256A3BU-AU</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Advanced Circuits</t>
+  </si>
+  <si>
+    <t>BH2AAA-W-ND</t>
+  </si>
+  <si>
+    <t>BH2AAAW</t>
+  </si>
+  <si>
+    <t>MPD</t>
+  </si>
+  <si>
+    <t>Battery Holder</t>
+  </si>
+  <si>
+    <t>use #2-56 button head cap screws (head 0.006" protrusion)</t>
+  </si>
+  <si>
+    <t>WM2900-ND</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>50-57-9402</t>
+  </si>
+  <si>
+    <t>WM1340-ND</t>
+  </si>
+  <si>
+    <t>Surface mount connector receptacle</t>
+  </si>
+  <si>
+    <t>Female connector housing for battery</t>
+  </si>
+  <si>
+    <t>EG5810CT-ND</t>
+  </si>
+  <si>
+    <t>Large switch</t>
+  </si>
+  <si>
+    <t>Crystal Oscillator</t>
+  </si>
+  <si>
+    <t>887-1274-1-ND</t>
+  </si>
+  <si>
+    <t>Crystal load capacitors</t>
+  </si>
+  <si>
+    <t>399-9344-1-ND</t>
+  </si>
+  <si>
+    <t>TXC</t>
+  </si>
+  <si>
+    <t>9C-16.000MEEJ-T</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>C1206C309D5GACTU</t>
+  </si>
+  <si>
+    <t>Large package for easy soldering; MCU XTAL1&amp;2 pin parasitic caps = 5.2pF and 6.8pF. Need 6pF additional to get to 18pF, so 3pF on each terminal. Doesn't account for trace capacitance.</t>
+  </si>
+  <si>
+    <t>Power Switch</t>
+  </si>
+  <si>
+    <t>401-1999-1-ND</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>JS102011SAQN</t>
+  </si>
+  <si>
+    <t>300mA max, should be OK with 8x20mA LEDs and MCU</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Pull-up resistor, 100K</t>
+  </si>
+  <si>
+    <t>311-100KFRCT-ND</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RC1206FR-07100KL</t>
+  </si>
+  <si>
+    <t>Filter capacitor, 0.1uF</t>
+  </si>
+  <si>
+    <t>311-1179-1-ND</t>
+  </si>
+  <si>
+    <t>CC1206KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>Filter capacitor, 10uF</t>
+  </si>
+  <si>
+    <t>311-1376-1-ND</t>
+  </si>
+  <si>
+    <t>CC1206ZKY5V7BB106</t>
+  </si>
+  <si>
+    <t>15-91-2025</t>
+  </si>
+  <si>
+    <t>Surface mount connector for UART</t>
+  </si>
+  <si>
+    <t>WM1341-ND</t>
+  </si>
+  <si>
+    <t>15-91-2035</t>
   </si>
 </sst>
 </file>
@@ -119,11 +296,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -439,23 +619,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699D6B1A-8ED7-4A49-A176-8E465F61A19C}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="167.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -463,47 +647,616 @@
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="I2" s="2">
         <v>7.2</v>
       </c>
-      <c r="F2" s="2">
-        <f>B2*E2</f>
+      <c r="J2" s="2">
+        <f>B2*I2</f>
         <v>7.2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G3" s="4"/>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J27" si="0">B3*I3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G4" s="4"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="I5" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>8</v>
       </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1206</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="0"/>
+        <v>3.04</v>
+      </c>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="I8" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G9" s="4"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="I10" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="I11" s="2">
+        <v>2.74</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="0"/>
+        <v>2.74</v>
+      </c>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="I12" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="I13" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1206</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="I16" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1206</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1206</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.38</v>
+      </c>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1206</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+      <c r="G21" s="4"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G23" s="4"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I25" s="2"/>
+      <c r="J25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I26" s="2"/>
+      <c r="J26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{5EFD6FDA-A680-43A6-A678-CD758D03BB9E}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{9B66B6C3-EECF-496D-BDA7-78D095CEC0DD}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5EFD6FDA-A680-43A6-A678-CD758D03BB9E}"/>
+    <hyperlink ref="D24" r:id="rId2" xr:uid="{9B66B6C3-EECF-496D-BDA7-78D095CEC0DD}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{61C9DB21-BC9D-46D4-A8DE-FA09AFBE8154}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{0A14FADA-9BF9-4FE9-8D26-06413B28F64D}"/>
+    <hyperlink ref="E22" r:id="rId5" xr:uid="{DE144B26-8656-4A66-BF65-E0D21617BDCA}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{B42C4F14-D203-4F68-BCE5-14603A7B1E5B}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{4CBA42B1-CA5B-47F0-85F7-559D74937A26}"/>
+    <hyperlink ref="D11" r:id="rId8" xr:uid="{53DA191B-0318-4B4C-BE10-CEB4FD7259E5}"/>
+    <hyperlink ref="D13" r:id="rId9" xr:uid="{772590EA-DF80-4E05-AD1B-FABB25FB08AF}"/>
+    <hyperlink ref="D14" r:id="rId10" xr:uid="{3E627C5D-0DD9-4189-8945-7A3513095285}"/>
+    <hyperlink ref="E8" r:id="rId11" xr:uid="{DFF55182-468F-45E3-8FF1-43BD1E16CFEA}"/>
+    <hyperlink ref="D16" r:id="rId12" xr:uid="{8C2996FD-9869-47E7-9499-E58C079466FE}"/>
+    <hyperlink ref="D18" r:id="rId13" xr:uid="{DEE5093B-180C-4E98-AD05-E3CD6E27551E}"/>
+    <hyperlink ref="D19" r:id="rId14" xr:uid="{1ACAD8CF-8565-4D18-9C6D-D706765A57E5}"/>
+    <hyperlink ref="D20" r:id="rId15" xr:uid="{31C5AFD6-4772-4F86-8A87-075D941CED8E}"/>
+    <hyperlink ref="D12" r:id="rId16" xr:uid="{B64C85DE-B608-46A1-9025-1C7EAD4C6945}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
continued adding footprints, etc.
</commit_message>
<xml_diff>
--- a/pcb/stereo-sync-pcb-bom.xlsx
+++ b/pcb/stereo-sync-pcb-bom.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f002r5k\GitHub\binary-counter\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE348F5A-5067-4A8B-AB78-67BCAD7169C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{BFAAAD16-CEC3-4355-83C2-768A17E1DB88}"/>
+    <workbookView xWindow="1176" yWindow="1176" windowWidth="21600" windowHeight="11328"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
   <si>
     <t>DigiKey Part</t>
   </si>
@@ -93,9 +92,6 @@
     <t>Microchip</t>
   </si>
   <si>
-    <t>Amphenol</t>
-  </si>
-  <si>
     <t>LTST-C150KRKT</t>
   </si>
   <si>
@@ -235,12 +231,39 @@
   </si>
   <si>
     <t>15-91-2035</t>
+  </si>
+  <si>
+    <t>SAM9026-ND</t>
+  </si>
+  <si>
+    <t>Right angle header, no shroud</t>
+  </si>
+  <si>
+    <t>1175-1864-ND</t>
+  </si>
+  <si>
+    <t>Shrouded keyed header</t>
+  </si>
+  <si>
+    <t>CNC Tech</t>
+  </si>
+  <si>
+    <t>3020-06-0300-00</t>
+  </si>
+  <si>
+    <t>Amphenol / FCI</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>TSM-103-01-L-DH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -269,7 +292,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +302,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -304,6 +333,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -618,28 +653,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699D6B1A-8ED7-4A49-A176-8E465F61A19C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="167.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="167.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -669,10 +704,10 @@
         <v>7</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
@@ -686,7 +721,7 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>3</v>
@@ -699,49 +734,84 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
       <c r="G3" s="4"/>
+      <c r="I3">
+        <v>0.48</v>
+      </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J27" si="0">B3*I3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G4" s="4"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="I4" s="8">
+        <v>0.88</v>
+      </c>
+      <c r="J4" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="I5" s="2">
+      <c r="G5" s="7"/>
+      <c r="I5" s="8">
         <v>0.36</v>
       </c>
-      <c r="J5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.36</v>
-      </c>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>8</v>
       </c>
@@ -752,10 +822,10 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="4">
         <v>1206</v>
@@ -769,7 +839,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G7" s="4"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2">
@@ -778,21 +848,21 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
         <v>26</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
       </c>
       <c r="G8" s="4"/>
       <c r="I8" s="2">
@@ -803,10 +873,10 @@
         <v>3.2</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G9" s="4"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2">
@@ -815,21 +885,21 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>33</v>
       </c>
       <c r="G10" s="4"/>
       <c r="I10" s="2">
@@ -841,21 +911,21 @@
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="4"/>
       <c r="I11" s="2">
@@ -867,21 +937,21 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="G12" s="4"/>
       <c r="I12" s="2">
@@ -893,21 +963,21 @@
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="G13" s="4"/>
       <c r="I13" s="2">
@@ -919,21 +989,21 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="G14" s="4">
         <v>1206</v>
@@ -946,10 +1016,10 @@
         <v>0.94</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -960,21 +1030,21 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" t="s">
         <v>49</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="G16" s="4"/>
       <c r="I16" s="2">
@@ -985,10 +1055,10 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -999,21 +1069,21 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" t="s">
         <v>55</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="G18" s="4">
         <v>1206</v>
@@ -1027,21 +1097,21 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="E19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G19" s="4">
         <v>1206</v>
@@ -1055,21 +1125,21 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="G20" s="4">
         <v>1206</v>
@@ -1083,7 +1153,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
       <c r="G21" s="4"/>
       <c r="I21" s="2"/>
@@ -1093,12 +1163,12 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G22" s="4"/>
       <c r="I22" s="2"/>
@@ -1108,7 +1178,7 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="G23" s="4"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2">
@@ -1117,7 +1187,7 @@
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>14</v>
       </c>
@@ -1132,7 +1202,7 @@
       </c>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="I25" s="2"/>
       <c r="J25" s="2">
         <f t="shared" si="0"/>
@@ -1140,7 +1210,7 @@
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="I26" s="2"/>
       <c r="J26" s="2">
         <f t="shared" si="0"/>
@@ -1148,12 +1218,12 @@
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2">
@@ -1162,101 +1232,103 @@
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{5EFD6FDA-A680-43A6-A678-CD758D03BB9E}"/>
-    <hyperlink ref="D24" r:id="rId2" xr:uid="{9B66B6C3-EECF-496D-BDA7-78D095CEC0DD}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{61C9DB21-BC9D-46D4-A8DE-FA09AFBE8154}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{0A14FADA-9BF9-4FE9-8D26-06413B28F64D}"/>
-    <hyperlink ref="E22" r:id="rId5" xr:uid="{DE144B26-8656-4A66-BF65-E0D21617BDCA}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{B42C4F14-D203-4F68-BCE5-14603A7B1E5B}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{4CBA42B1-CA5B-47F0-85F7-559D74937A26}"/>
-    <hyperlink ref="D11" r:id="rId8" xr:uid="{53DA191B-0318-4B4C-BE10-CEB4FD7259E5}"/>
-    <hyperlink ref="D13" r:id="rId9" xr:uid="{772590EA-DF80-4E05-AD1B-FABB25FB08AF}"/>
-    <hyperlink ref="D14" r:id="rId10" xr:uid="{3E627C5D-0DD9-4189-8945-7A3513095285}"/>
-    <hyperlink ref="E8" r:id="rId11" xr:uid="{DFF55182-468F-45E3-8FF1-43BD1E16CFEA}"/>
-    <hyperlink ref="D16" r:id="rId12" xr:uid="{8C2996FD-9869-47E7-9499-E58C079466FE}"/>
-    <hyperlink ref="D18" r:id="rId13" xr:uid="{DEE5093B-180C-4E98-AD05-E3CD6E27551E}"/>
-    <hyperlink ref="D19" r:id="rId14" xr:uid="{1ACAD8CF-8565-4D18-9C6D-D706765A57E5}"/>
-    <hyperlink ref="D20" r:id="rId15" xr:uid="{31C5AFD6-4772-4F86-8A87-075D941CED8E}"/>
-    <hyperlink ref="D12" r:id="rId16" xr:uid="{B64C85DE-B608-46A1-9025-1C7EAD4C6945}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D24" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="E22" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D13" r:id="rId9"/>
+    <hyperlink ref="D14" r:id="rId10"/>
+    <hyperlink ref="E8" r:id="rId11"/>
+    <hyperlink ref="D16" r:id="rId12"/>
+    <hyperlink ref="D18" r:id="rId13"/>
+    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId15"/>
+    <hyperlink ref="D12" r:id="rId16"/>
+    <hyperlink ref="D4" r:id="rId17"/>
+    <hyperlink ref="D3" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished adding footprints and started laying out board
</commit_message>
<xml_diff>
--- a/pcb/stereo-sync-pcb-bom.xlsx
+++ b/pcb/stereo-sync-pcb-bom.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f002r5k\GitHub\binary-counter\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D17DB2-3A3B-40FD-A534-7418D30619F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1176" yWindow="1176" windowWidth="21600" windowHeight="11328"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
   <si>
     <t>DigiKey Part</t>
   </si>
@@ -56,9 +57,6 @@
     <t>Extended</t>
   </si>
   <si>
-    <t>1080-1184-ND</t>
-  </si>
-  <si>
     <t>609-6366-ND</t>
   </si>
   <si>
@@ -74,9 +72,6 @@
     <t>MCU</t>
   </si>
   <si>
-    <t>LED Array</t>
-  </si>
-  <si>
     <t>Programming header</t>
   </si>
   <si>
@@ -140,12 +135,6 @@
     <t>Female connector housing for battery</t>
   </si>
   <si>
-    <t>EG5810CT-ND</t>
-  </si>
-  <si>
-    <t>Large switch</t>
-  </si>
-  <si>
     <t>Crystal Oscillator</t>
   </si>
   <si>
@@ -258,12 +247,24 @@
   </si>
   <si>
     <t>TSM-103-01-L-DH</t>
+  </si>
+  <si>
+    <t>Resistor, 47R0</t>
+  </si>
+  <si>
+    <t>311-47.0FRCT-ND</t>
+  </si>
+  <si>
+    <t>RC1206FR-0747RL</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -292,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +312,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -325,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -339,6 +346,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -653,28 +661,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="24.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="167.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="167.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -682,16 +690,16 @@
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
@@ -704,24 +712,24 @@
         <v>7</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>3</v>
@@ -734,46 +742,46 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G3" s="4"/>
       <c r="I3">
         <v>0.48</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J27" si="0">B3*I3</f>
+        <f t="shared" ref="J3:J18" si="0">B3*I3</f>
         <v>0.48</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G4" s="7"/>
       <c r="I4" s="8">
@@ -785,21 +793,21 @@
       </c>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="7"/>
       <c r="I5" s="8">
@@ -811,21 +819,21 @@
       </c>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" s="4">
         <v>1206</v>
@@ -839,79 +847,113 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
       <c r="G7" s="4"/>
-      <c r="I7" s="2"/>
+      <c r="I7" s="2">
+        <v>3.2</v>
+      </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3.2</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
+      <c r="E8" t="s">
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G8" s="4"/>
       <c r="I8" s="2">
-        <v>3.2</v>
+        <v>0.27</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="K8" s="2" t="s">
+        <v>0.27</v>
+      </c>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F9" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="G9" s="4"/>
-      <c r="I9" s="2"/>
+      <c r="I9" s="2">
+        <v>2.74</v>
+      </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.74</v>
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="G10" s="4"/>
       <c r="I10" s="2">
-        <v>0.27</v>
+        <v>3.6</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>0.27</v>
+        <v>3.6</v>
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>1</v>
       </c>
@@ -919,414 +961,342 @@
         <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="G11" s="4"/>
       <c r="I11" s="2">
-        <v>2.74</v>
+        <v>0.59</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>2.74</v>
+        <v>0.59</v>
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1206</v>
+      </c>
       <c r="I12" s="2">
-        <v>3.6</v>
+        <v>0.47</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.94</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G13" s="4"/>
       <c r="I13" s="2">
-        <v>0.59</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
-        <v>0.59</v>
-      </c>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="G14" s="4">
         <v>1206</v>
       </c>
       <c r="I14" s="2">
-        <v>0.47</v>
+        <v>0.1</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="0"/>
-        <v>0.94</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D15" s="1"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="I15" s="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1206</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.19</v>
+      </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1206</v>
+      </c>
       <c r="I16" s="2">
-        <v>0.56000000000000005</v>
+        <v>0.3</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="0"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="K16" s="2" t="s">
+        <v>0.3</v>
+      </c>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D17" s="1"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="I17" s="2"/>
+      <c r="F17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1206</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.1</v>
+      </c>
       <c r="J17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="4">
-        <v>1206</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="4"/>
       <c r="I18" s="2">
-        <v>0.1</v>
+        <v>33</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>99</v>
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="4">
-        <v>1206</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="J19" s="2">
-        <f t="shared" si="0"/>
-        <v>0.38</v>
-      </c>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G19" s="4"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="4">
-        <v>1206</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="J20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="G20" s="4"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D21" s="1"/>
-      <c r="G21" s="4"/>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I21" s="2"/>
-      <c r="J21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I22" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" s="9">
+        <f>SUM(J2:J21)</f>
+        <v>123.2</v>
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G23" s="4"/>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I23" s="2"/>
-      <c r="J23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="4"/>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I24" s="2"/>
-      <c r="J24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I25" s="2"/>
-      <c r="J25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I26" s="2"/>
-      <c r="J26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" t="s">
-        <v>36</v>
-      </c>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I27" s="2"/>
-      <c r="J27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D24" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4"/>
-    <hyperlink ref="E22" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D10" r:id="rId7"/>
-    <hyperlink ref="D11" r:id="rId8"/>
-    <hyperlink ref="D13" r:id="rId9"/>
-    <hyperlink ref="D14" r:id="rId10"/>
-    <hyperlink ref="E8" r:id="rId11"/>
-    <hyperlink ref="D16" r:id="rId12"/>
-    <hyperlink ref="D18" r:id="rId13"/>
-    <hyperlink ref="D19" r:id="rId14"/>
-    <hyperlink ref="D20" r:id="rId15"/>
-    <hyperlink ref="D12" r:id="rId16"/>
-    <hyperlink ref="D4" r:id="rId17"/>
-    <hyperlink ref="D3" r:id="rId18"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E18" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D4" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D3" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D17" r:id="rId18" xr:uid="{7C4773B0-4C80-411C-96FC-8BD160D04832}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
continued PCB layout, all components in appropriate locations now
</commit_message>
<xml_diff>
--- a/pcb/stereo-sync-pcb-bom.xlsx
+++ b/pcb/stereo-sync-pcb-bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f002r5k\GitHub\binary-counter\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D17DB2-3A3B-40FD-A534-7418D30619F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D9BD37-1738-469D-A631-138106B32E62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
   <si>
     <t>DigiKey Part</t>
   </si>
@@ -259,6 +259,51 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Test Point</t>
+  </si>
+  <si>
+    <t>36-5000-ND</t>
+  </si>
+  <si>
+    <t>Keystone</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>D1-D8</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>XTAL1</t>
+  </si>
+  <si>
+    <t>C4-C5</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>C1,C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>R2-R9</t>
+  </si>
+  <si>
+    <t>TP1-3</t>
   </si>
 </sst>
 </file>
@@ -319,7 +364,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -327,26 +372,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -662,627 +728,707 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="167.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="167.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="2">
+      <c r="H2" s="6"/>
+      <c r="I2" s="9">
         <v>7.2</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="9">
         <f>B2*I2</f>
         <v>7.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="I3">
+      <c r="G3" s="8"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6">
         <v>0.48</v>
       </c>
-      <c r="J3" s="2">
-        <f t="shared" ref="J3:J18" si="0">B3*I3</f>
+      <c r="J3" s="9">
+        <f t="shared" ref="J3:J19" si="0">B3*I3</f>
         <v>0.48</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="10">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="I4" s="8">
+      <c r="G4" s="12"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="13">
         <v>0.88</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="10">
         <v>0</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="I5" s="8">
+      <c r="G5" s="12"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="13">
         <v>0.36</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="6">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="8">
         <v>1206</v>
       </c>
-      <c r="I6" s="2">
+      <c r="H6" s="6"/>
+      <c r="I6" s="9">
         <v>0.38</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="9">
         <f t="shared" si="0"/>
         <v>3.04</v>
       </c>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="I7" s="2">
+      <c r="G7" s="8"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="9">
         <v>3.2</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="9">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="I8" s="2">
+      <c r="G8" s="8"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="9">
         <v>0.27</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="9">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="I9" s="2">
+      <c r="G9" s="8"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="9">
         <v>2.74</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="9">
         <f t="shared" si="0"/>
         <v>2.74</v>
       </c>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="I10" s="2">
+      <c r="G10" s="12"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="13">
         <v>3.6</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="13">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="K10" s="13"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="I11" s="2">
+      <c r="G11" s="8"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="9">
         <v>0.59</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="9">
         <f t="shared" si="0"/>
         <v>0.59</v>
       </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="8">
         <v>1206</v>
       </c>
-      <c r="I12" s="2">
+      <c r="H12" s="6"/>
+      <c r="I12" s="9">
         <v>0.47</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="9">
         <f t="shared" si="0"/>
         <v>0.94</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="6">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="I13" s="2">
+      <c r="G13" s="8"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="9">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="9">
         <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="6">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="8">
         <v>1206</v>
       </c>
-      <c r="I14" s="2">
+      <c r="H14" s="6"/>
+      <c r="I14" s="9">
         <v>0.1</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="6">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="8">
         <v>1206</v>
       </c>
-      <c r="I15" s="2">
+      <c r="H15" s="6"/>
+      <c r="I15" s="9">
         <v>0.19</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="9">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="8">
         <v>1206</v>
       </c>
-      <c r="I16" s="2">
+      <c r="H16" s="6"/>
+      <c r="I16" s="9">
         <v>0.3</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="9">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="6">
         <v>8</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="8">
         <v>1206</v>
       </c>
-      <c r="I17" s="2">
+      <c r="H17" s="6"/>
+      <c r="I17" s="9">
         <v>0.1</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="9">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="8">
+        <v>5000</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="9">
+        <v>0.35</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6">
+        <v>3</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="I18" s="2">
+      <c r="F19" s="6"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="9">
         <v>33</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J19" s="9">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G19" s="4"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D20" s="1"/>
-      <c r="G20" s="4"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I22" s="9" t="s">
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G20" s="2"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I21" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J22" s="9">
-        <f>SUM(J2:J21)</f>
-        <v>123.2</v>
-      </c>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+      <c r="J21" s="4">
+        <f>SUM(J2:J20)</f>
+        <v>124.25</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="D6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E18" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E19" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="D8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="D9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
@@ -1297,8 +1443,9 @@
     <hyperlink ref="D4" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="D3" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="D17" r:id="rId18" xr:uid="{7C4773B0-4C80-411C-96FC-8BD160D04832}"/>
+    <hyperlink ref="D18" r:id="rId19" xr:uid="{7A0693B9-81D7-4D3E-B303-B88FE6D39E52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added schematic notes, changed R2-9 to 27R0 to accomodate I/O pin input impedance
</commit_message>
<xml_diff>
--- a/pcb/stereo-sync-pcb-bom.xlsx
+++ b/pcb/stereo-sync-pcb-bom.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f002r5k\GitHub\binary-counter\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8224A76-4CC2-471F-A7AD-AE9459FD285A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
   <si>
     <t>DigiKey Part</t>
   </si>
@@ -248,15 +249,6 @@
     <t>TSM-103-01-L-DH</t>
   </si>
   <si>
-    <t>Resistor, 47R0</t>
-  </si>
-  <si>
-    <t>311-47.0FRCT-ND</t>
-  </si>
-  <si>
-    <t>RC1206FR-0747RL</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -312,12 +304,24 @@
   </si>
   <si>
     <t>J3</t>
+  </si>
+  <si>
+    <t>Resistor, 27R0</t>
+  </si>
+  <si>
+    <t>311-27ERCT-ND</t>
+  </si>
+  <si>
+    <t>RC1206JR-0727RL</t>
+  </si>
+  <si>
+    <t>27 ohm should sink ~17mA max from LED into micro; max spec on Xmega pins is 20mA (25mA absolute max), effective 30ohm impedance to sink per datasheet graph, LED drops ~2.0V for 10-25mA, assuming max supply 3.0V, may sink 21mA transiently with new batteries if each provides 1.6V at load current (unlikely)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -400,27 +404,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -735,751 +783,777 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="24.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="167.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="105.7109375" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="5">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="8">
+      <c r="H2" s="6"/>
+      <c r="I2" s="4">
         <v>7.2</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="4">
         <f>B2*I2</f>
         <v>7.2</v>
       </c>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="5">
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5">
+      <c r="G3" s="13"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6">
         <v>0.48</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="4">
         <f t="shared" ref="J3:J20" si="0">B3*I3</f>
         <v>0.48</v>
       </c>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="14">
         <v>0</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="12">
+      <c r="G4" s="16"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="7">
         <v>0.88</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="9">
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="14">
         <v>0</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="12">
+      <c r="G5" s="16"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="7">
         <v>0.36</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="5">
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="6">
         <v>8</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="13">
         <v>1206</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="8">
+      <c r="H6" s="6"/>
+      <c r="I6" s="4">
         <v>0.38</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="4">
         <f t="shared" si="0"/>
         <v>3.04</v>
       </c>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5">
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8">
+      <c r="G7" s="13"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="4">
         <v>3.2</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="4">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="8">
+      <c r="G8" s="13"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="4">
         <v>0.27</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="4">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="5">
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="8">
+      <c r="G9" s="13"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="4">
         <v>2.74</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="4">
         <f t="shared" si="0"/>
         <v>2.74</v>
       </c>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9">
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14">
         <v>1</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="12">
+      <c r="G10" s="16"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="7">
         <v>3.6</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="7">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="5">
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="8">
+      <c r="G11" s="13"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="4">
         <v>0.59</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="4">
         <f t="shared" si="0"/>
         <v>0.59</v>
       </c>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="5">
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="13">
         <v>1206</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="8">
+      <c r="H12" s="6"/>
+      <c r="I12" s="4">
         <v>0.47</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="4">
         <f t="shared" si="0"/>
         <v>0.94</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="5">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="6">
         <v>1</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="8">
+      <c r="G13" s="13"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="4">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="4">
         <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="5">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="6">
         <v>1</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="13">
         <v>1206</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="8">
+      <c r="H14" s="6"/>
+      <c r="I14" s="4">
         <v>0.1</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="4">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="5">
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="6">
         <v>2</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="13">
         <v>1206</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="8">
+      <c r="H15" s="6"/>
+      <c r="I15" s="4">
         <v>0.19</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="4">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
-      <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="5">
+      <c r="K15" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="13">
         <v>1206</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="8">
+      <c r="H16" s="6"/>
+      <c r="I16" s="4">
         <v>0.3</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="4">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="5">
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="6">
         <v>8</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="C17" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="7">
+      <c r="F17" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="13">
         <v>1206</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="8">
+      <c r="H17" s="6"/>
+      <c r="I17" s="4">
         <v>0.1</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="4">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="5">
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="C18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="13">
         <v>5000</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="8">
+      <c r="G18" s="13"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="4">
         <v>0.35</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="4">
         <f t="shared" si="0"/>
         <v>1.0499999999999998</v>
       </c>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5">
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6">
         <v>1</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="8">
+      <c r="C19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="4">
         <f>10*2.5*1</f>
         <v>25</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="4">
         <f>B19*I19</f>
         <v>25</v>
       </c>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9">
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14">
         <v>0</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10" t="s">
+      <c r="D20" s="14"/>
+      <c r="E20" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="12">
+      <c r="F20" s="14"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="7">
         <v>33</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G21" s="2"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J22" s="4">
+      <c r="K20" s="10"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="J22" s="21">
         <f>SUM(J2:J21)</f>
         <v>50.25</v>
       </c>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-    </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="20"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2"/>
-    <hyperlink ref="D6" r:id="rId3"/>
-    <hyperlink ref="E20" r:id="rId4"/>
-    <hyperlink ref="D7" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="D11" r:id="rId8"/>
-    <hyperlink ref="D12" r:id="rId9"/>
-    <hyperlink ref="E7" r:id="rId10"/>
-    <hyperlink ref="D13" r:id="rId11"/>
-    <hyperlink ref="D14" r:id="rId12"/>
-    <hyperlink ref="D15" r:id="rId13"/>
-    <hyperlink ref="D16" r:id="rId14"/>
-    <hyperlink ref="D10" r:id="rId15"/>
-    <hyperlink ref="D4" r:id="rId16"/>
-    <hyperlink ref="D3" r:id="rId17"/>
-    <hyperlink ref="D17" r:id="rId18"/>
-    <hyperlink ref="D18" r:id="rId19"/>
-    <hyperlink ref="E19" r:id="rId20"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E20" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D4" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D3" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D17" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D18" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E19" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId21"/>

</xml_diff>